<commit_message>
Old Latex for Free-Stream Velocity
</commit_message>
<xml_diff>
--- a/C10/origins.xlsx
+++ b/C10/origins.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smtgn\Desktop\S19\Thermal Fluids\GitHub\24321-A4\C10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/PKBACK# 001/GitHub/24321-A4/C10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{100A1921-83C7-4BBD-97DC-26A9BBA5E967}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE44022-809D-474B-8F54-B6EEF2B6D89E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{5625920C-C6DC-40A4-AED5-A96A29664ECF}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19400" windowHeight="10400" activeTab="1" xr2:uid="{5625920C-C6DC-40A4-AED5-A96A29664ECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Fig1b</t>
   </si>
@@ -70,6 +71,9 @@
   </si>
   <si>
     <t>Image W</t>
+  </si>
+  <si>
+    <t>+/-</t>
   </si>
 </sst>
 </file>
@@ -105,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,21 +428,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB01572F-5288-47ED-9871-99B42C50866A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.62890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -457,7 +461,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -477,7 +481,7 @@
         <v>4032</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -498,7 +502,7 @@
         <v>3297</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -519,7 +523,7 @@
         <v>4032</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -540,7 +544,7 @@
         <v>3910</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -561,7 +565,7 @@
         <v>3886</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -582,7 +586,7 @@
         <v>4032</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -603,7 +607,7 @@
         <v>4032</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -624,7 +628,7 @@
         <v>4030</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -643,6 +647,233 @@
       </c>
       <c r="F10">
         <v>3645</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EE6774-E6B9-3A42-A2D0-5D22EB6D589D}">
+  <dimension ref="A2:P10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>459</v>
+      </c>
+      <c r="B2">
+        <f>A3</f>
+        <v>545</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:P2" si="0">B3</f>
+        <v>667</v>
+      </c>
+      <c r="D2">
+        <f>C3</f>
+        <v>766</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>865</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>967</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>1069</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>1166</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>1257</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>1346</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>1442</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>1554</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>1630</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>1746</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>1852</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="0"/>
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>545</v>
+      </c>
+      <c r="B3">
+        <v>667</v>
+      </c>
+      <c r="C3">
+        <v>766</v>
+      </c>
+      <c r="D3">
+        <v>865</v>
+      </c>
+      <c r="E3">
+        <v>967</v>
+      </c>
+      <c r="F3">
+        <v>1069</v>
+      </c>
+      <c r="G3">
+        <v>1166</v>
+      </c>
+      <c r="H3">
+        <v>1257</v>
+      </c>
+      <c r="I3">
+        <v>1346</v>
+      </c>
+      <c r="J3">
+        <v>1442</v>
+      </c>
+      <c r="K3">
+        <v>1554</v>
+      </c>
+      <c r="L3">
+        <v>1630</v>
+      </c>
+      <c r="M3">
+        <v>1746</v>
+      </c>
+      <c r="N3">
+        <v>1852</v>
+      </c>
+      <c r="O3">
+        <v>1962</v>
+      </c>
+      <c r="P3">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>A3-A2</f>
+        <v>86</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:P4" si="1">B3-B2</f>
+        <v>122</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f>AVERAGE(A4:P4)</f>
+        <v>99.3125</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <f>STDEV(A4:P4)</f>
+        <v>12.158501826568381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f>2*C6/A6</f>
+        <v>0.24485340368167915</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>9.68/A6</f>
+        <v>9.7470106985525481E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f>A9*206</f>
+        <v>20.078842039018248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cylinder Table 1 Data
</commit_message>
<xml_diff>
--- a/C10/origins.xlsx
+++ b/C10/origins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/PKBACK# 001/GitHub/24321-A4/C10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE44022-809D-474B-8F54-B6EEF2B6D89E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6653D5-A7A2-964C-BD4D-F3CF9FEFDF53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19400" windowHeight="10400" activeTab="1" xr2:uid="{5625920C-C6DC-40A4-AED5-A96A29664ECF}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19400" windowHeight="10400" xr2:uid="{5625920C-C6DC-40A4-AED5-A96A29664ECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,34 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Fig1b</t>
-  </si>
-  <si>
-    <t>Fib2</t>
-  </si>
-  <si>
-    <t>Fig4</t>
-  </si>
-  <si>
-    <t>Fig5</t>
-  </si>
-  <si>
-    <t>Fig6</t>
-  </si>
-  <si>
-    <t>Fig7</t>
-  </si>
-  <si>
-    <t>Fig8</t>
-  </si>
-  <si>
-    <t>Fig9</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Square Size</t>
   </si>
@@ -64,9 +37,6 @@
     <t>Origin Y</t>
   </si>
   <si>
-    <t>Fig10</t>
-  </si>
-  <si>
     <t>Image H</t>
   </si>
   <si>
@@ -74,6 +44,9 @@
   </si>
   <si>
     <t>+/-</t>
+  </si>
+  <si>
+    <t>Figure</t>
   </si>
 </sst>
 </file>
@@ -428,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB01572F-5288-47ED-9871-99B42C50866A}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="F12:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -443,27 +416,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>206</v>
@@ -482,8 +455,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
         <f>(108.5+112)/2</f>
@@ -503,8 +476,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="A4">
+        <v>4</v>
       </c>
       <c r="B4">
         <f>(189+195.5)/2</f>
@@ -524,8 +497,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="A5">
+        <v>5</v>
       </c>
       <c r="B5">
         <f>(150+146)/2</f>
@@ -545,8 +518,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A6">
+        <v>6</v>
       </c>
       <c r="B6">
         <f>(171.5+166.6)/2</f>
@@ -566,8 +539,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
+      <c r="A7">
+        <v>7</v>
       </c>
       <c r="B7">
         <f>(159+152.5)/2</f>
@@ -587,8 +560,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
+      <c r="A8">
+        <v>8</v>
       </c>
       <c r="B8">
         <f>(167.5+160.5)</f>
@@ -608,8 +581,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
+      <c r="A9">
+        <v>9</v>
       </c>
       <c r="B9">
         <f>(139+132.5)/2</f>
@@ -629,8 +602,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
+      <c r="A10">
+        <v>10</v>
       </c>
       <c r="B10">
         <f>(131+136)/2</f>
@@ -651,6 +624,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -658,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EE6774-E6B9-3A42-A2D0-5D22EB6D589D}">
   <dimension ref="A2:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -851,7 +825,7 @@
         <v>99.3125</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <f>STDEV(A4:P4)</f>

</xml_diff>